<commit_message>
add the time management
</commit_message>
<xml_diff>
--- a/recorded.xlsx
+++ b/recorded.xlsx
@@ -16,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="285">
   <si>
     <t xml:space="preserve">                                                                       Note</t>
   </si>
@@ -876,6 +876,105 @@
   </si>
   <si>
     <t>S:人大蓝微</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>十二月十七号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>在家编产品编号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>十二月十八号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>见二师兄，一起学习，lentern,chrome,输入法，计算机概论，日语第八课</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>十二月十九号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>在家上传产品到国际站</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>十二月二十号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>北邮漫咖啡</t>
+  </si>
+  <si>
+    <t>上传产品，定去葫芦岛行程</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>十二月二十一号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>茶馆</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传产品</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>十二月二十二号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>北邮</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>和哈立德一起出发</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>十二月二十三号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>辽工大</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>见院长浅谈只会矿山项目</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>古城</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>等院长，见了书记，老师，同学</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>—二十五号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>十二月二十六号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>更改完</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>更改产品信息（40个产品）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人工作时间记录</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1227,15 +1326,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R147"/>
+  <dimension ref="A1:R159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="C148" sqref="C148"/>
+    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="A157" sqref="A157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
     <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.375" customWidth="1"/>
     <col min="4" max="4" width="60.875" customWidth="1"/>
@@ -2902,12 +3001,12 @@
         <v>255</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.15">
       <c r="C145" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A146" t="s">
         <v>257</v>
       </c>
@@ -2918,12 +3017,144 @@
         <v>258</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B147" s="1">
         <v>0.52083333333333337</v>
       </c>
       <c r="C147" t="s">
         <v>259</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A148" t="s">
+        <v>260</v>
+      </c>
+      <c r="C148" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A149" t="s">
+        <v>262</v>
+      </c>
+      <c r="B149" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C149" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A150" t="s">
+        <v>264</v>
+      </c>
+      <c r="C150" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A151" t="s">
+        <v>266</v>
+      </c>
+      <c r="B151" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C151" t="s">
+        <v>267</v>
+      </c>
+      <c r="D151" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A152" t="s">
+        <v>269</v>
+      </c>
+      <c r="B152" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C152" t="s">
+        <v>270</v>
+      </c>
+      <c r="D152" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A153" t="s">
+        <v>272</v>
+      </c>
+      <c r="B153" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C153" t="s">
+        <v>273</v>
+      </c>
+      <c r="D153" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B154" s="1">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="C154" t="s">
+        <v>276</v>
+      </c>
+      <c r="D154" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A155" t="s">
+        <v>275</v>
+      </c>
+      <c r="B155" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C155" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A156" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B156" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C156" t="s">
+        <v>276</v>
+      </c>
+      <c r="D156" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A157" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A158" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B158" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B159" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -2932,6 +3163,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>